<commit_message>
Fixed typo in axis
</commit_message>
<xml_diff>
--- a/Ch12_Math/Averaging.xlsx
+++ b/Ch12_Math/Averaging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eleci\work\oreilly\git\Ch12_Math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE451DB-BC68-47A1-8508-288ECF93F241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C0199E-3767-4DE4-8CA4-B82EA0D12B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{CBBFF73D-5E74-4E12-A2B5-9B008E957599}"/>
+    <workbookView xWindow="12500" yWindow="2470" windowWidth="23080" windowHeight="12510" xr2:uid="{CBBFF73D-5E74-4E12-A2B5-9B008E957599}"/>
   </bookViews>
   <sheets>
     <sheet name="different averages" sheetId="1" r:id="rId1"/>
@@ -1377,7 +1377,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Rolling and block averaves</a:t>
+                  <a:t>Rolling and block averages</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4820,8 +4820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B24C9F1-626B-4ACB-8BDB-12377A6560F9}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6111,7 +6111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C826B7F-2D63-4BC9-B44F-54E74CA719C9}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>